<commit_message>
Added NDR rule numbers to tests
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="222">
   <si>
     <t>Add</t>
   </si>
@@ -584,9 +584,6 @@
     <t>Bad reference</t>
   </si>
   <si>
-    <t>A CSC type with a "CodeSimpleType" base must be named similarly, with the name ending in "CodeType".</t>
-  </si>
-  <si>
     <t>type-name-codeType-inconsistent</t>
   </si>
   <si>
@@ -635,12 +632,6 @@
     <t>A facet must belong to a simple type.</t>
   </si>
   <si>
-    <t>A facet must have a qualified type name.</t>
-  </si>
-  <si>
-    <t>A facet must have a valid qualified type name.</t>
-  </si>
-  <si>
     <t>facet-name-all-complex</t>
   </si>
   <si>
@@ -656,13 +647,49 @@
     <t>An enumeration must have a definition.</t>
   </si>
   <si>
-    <t>Optional: It can be useful to provide definitions for patterns.</t>
-  </si>
-  <si>
     <t>Patterns</t>
   </si>
   <si>
     <t>info</t>
+  </si>
+  <si>
+    <t>9-10, 9-25</t>
+  </si>
+  <si>
+    <t>10-18</t>
+  </si>
+  <si>
+    <t>A CSC type with a "CodeSimpleType" base should be named similarly, with the name ending in "CodeType".</t>
+  </si>
+  <si>
+    <t>10-49</t>
+  </si>
+  <si>
+    <t>9-12, 9-26</t>
+  </si>
+  <si>
+    <t>11-44, 11-45</t>
+  </si>
+  <si>
+    <t>Optional: A pattern should have a definition.</t>
+  </si>
+  <si>
+    <t>9-14</t>
+  </si>
+  <si>
+    <t>A facet must have a type name.</t>
+  </si>
+  <si>
+    <t>A facet must have a type namespace prefix.</t>
+  </si>
+  <si>
+    <t>A facet must have a valid type namespace prefix.</t>
+  </si>
+  <si>
+    <t>A facet must have a valid type name.</t>
+  </si>
+  <si>
+    <t>11-7, 11-8</t>
   </si>
 </sst>
 </file>
@@ -771,6 +798,40 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="52">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1154,40 +1215,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1205,22 +1232,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P114" totalsRowShown="0">
   <autoFilter ref="A1:P114"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="ID" dataDxfId="51"/>
-    <tableColumn id="10" name="Description" dataDxfId="50"/>
-    <tableColumn id="17" name="Category" dataDxfId="49"/>
-    <tableColumn id="16" name="NDR" dataDxfId="48"/>
+    <tableColumn id="1" name="ID" dataDxfId="10"/>
+    <tableColumn id="10" name="Description" dataDxfId="9"/>
+    <tableColumn id="17" name="Category" dataDxfId="8"/>
+    <tableColumn id="16" name="NDR" dataDxfId="7"/>
     <tableColumn id="2" name="Component"/>
     <tableColumn id="3" name="Field"/>
     <tableColumn id="14" name="Applicability"/>
     <tableColumn id="11" name="Location"/>
     <tableColumn id="9" name="Severity"/>
-    <tableColumn id="4" name="Add" dataDxfId="47"/>
-    <tableColumn id="5" name="Edit" dataDxfId="46"/>
-    <tableColumn id="6" name="Delete" dataDxfId="45"/>
-    <tableColumn id="13" name="Clear" dataDxfId="44"/>
-    <tableColumn id="7" name="Map" dataDxfId="43"/>
-    <tableColumn id="8" name="Subset" dataDxfId="42"/>
-    <tableColumn id="15" name="Exceptions" dataDxfId="41"/>
+    <tableColumn id="4" name="Add" dataDxfId="6"/>
+    <tableColumn id="5" name="Edit" dataDxfId="5"/>
+    <tableColumn id="6" name="Delete" dataDxfId="4"/>
+    <tableColumn id="13" name="Clear" dataDxfId="3"/>
+    <tableColumn id="7" name="Map" dataDxfId="2"/>
+    <tableColumn id="8" name="Subset" dataDxfId="1"/>
+    <tableColumn id="15" name="Exceptions" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3316,7 +3343,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>153</v>
@@ -3346,7 +3373,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>59</v>
@@ -3354,6 +3381,9 @@
       <c r="C61" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D61" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E61" t="s">
         <v>6</v>
       </c>
@@ -3391,7 +3421,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>23</v>
@@ -3399,6 +3429,9 @@
       <c r="C62" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D62" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="E62" t="s">
         <v>6</v>
       </c>
@@ -3436,16 +3469,16 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="E63" t="s">
         <v>6</v>
@@ -3623,6 +3656,9 @@
       <c r="C67" s="3" t="s">
         <v>150</v>
       </c>
+      <c r="D67" s="6" t="s">
+        <v>221</v>
+      </c>
       <c r="E67" t="s">
         <v>6</v>
       </c>
@@ -3836,6 +3872,9 @@
       <c r="C72" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D72" s="6" t="s">
+        <v>210</v>
+      </c>
       <c r="E72" t="s">
         <v>6</v>
       </c>
@@ -3849,7 +3888,7 @@
         <v>39</v>
       </c>
       <c r="I72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>169</v>
@@ -3873,13 +3912,16 @@
     </row>
     <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E73" t="s">
         <v>6</v>
@@ -3894,7 +3936,7 @@
         <v>39</v>
       </c>
       <c r="I73" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>169</v>
@@ -3911,6 +3953,9 @@
       <c r="C74" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="D74" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="E74" t="s">
         <v>6</v>
       </c>
@@ -3956,6 +4001,9 @@
       <c r="C75" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D75" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E75" t="s">
         <v>6</v>
       </c>
@@ -4001,6 +4049,9 @@
       <c r="C76" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D76" s="6" t="s">
+        <v>212</v>
+      </c>
       <c r="E76" t="s">
         <v>6</v>
       </c>
@@ -4091,6 +4142,9 @@
       <c r="C78" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D78" s="6" t="s">
+        <v>213</v>
+      </c>
       <c r="E78" t="s">
         <v>6</v>
       </c>
@@ -4136,6 +4190,9 @@
       <c r="C79" s="3" t="s">
         <v>148</v>
       </c>
+      <c r="D79" s="6" t="s">
+        <v>214</v>
+      </c>
       <c r="E79" t="s">
         <v>6</v>
       </c>
@@ -4218,13 +4275,16 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E81" t="s">
         <v>6</v>
@@ -4256,6 +4316,9 @@
       <c r="C82" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D82" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E82" t="s">
         <v>6</v>
       </c>
@@ -4427,6 +4490,9 @@
       <c r="C86" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D86" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E86" t="s">
         <v>6</v>
       </c>
@@ -4472,6 +4538,9 @@
       <c r="C87" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D87" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E87" t="s">
         <v>6</v>
       </c>
@@ -4502,6 +4571,9 @@
       <c r="C88" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D88" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E88" t="s">
         <v>6</v>
       </c>
@@ -4546,6 +4618,9 @@
       </c>
       <c r="C89" s="3" t="s">
         <v>185</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E89" t="s">
         <v>6</v>
@@ -5134,13 +5209,16 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E104" t="s">
         <v>12</v>
@@ -5167,10 +5245,13 @@
         <v>167</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E105" t="s">
         <v>12</v>
@@ -5209,14 +5290,17 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D106" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E106" t="s">
         <v>12</v>
       </c>
@@ -5239,13 +5323,16 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E107" t="s">
         <v>12</v>
@@ -5284,13 +5371,16 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E108" t="s">
         <v>12</v>
@@ -5314,13 +5404,16 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E109" t="s">
         <v>12</v>
@@ -5329,7 +5422,7 @@
         <v>65</v>
       </c>
       <c r="G109" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H109" t="s">
         <v>39</v>
@@ -5352,6 +5445,9 @@
       <c r="C110" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D110" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E110" t="s">
         <v>12</v>
       </c>
@@ -5389,7 +5485,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>82</v>
@@ -5397,6 +5493,9 @@
       <c r="C111" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D111" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E111" t="s">
         <v>12</v>
       </c>
@@ -5434,14 +5533,17 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D112" s="6" t="s">
+        <v>216</v>
+      </c>
       <c r="E112" t="s">
         <v>12</v>
       </c>
@@ -5449,7 +5551,7 @@
         <v>63</v>
       </c>
       <c r="G112" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H112" t="s">
         <v>39</v>
@@ -5477,16 +5579,19 @@
       </c>
       <c r="P112" s="1"/>
     </row>
-    <row r="113" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D113" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E113" t="s">
         <v>12</v>
       </c>
@@ -5494,13 +5599,13 @@
         <v>63</v>
       </c>
       <c r="G113" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H113" t="s">
         <v>39</v>
       </c>
       <c r="I113" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J113" s="1" t="s">
         <v>169</v>
@@ -5532,6 +5637,9 @@
       <c r="C114" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D114" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E114" t="s">
         <v>12</v>
       </c>
@@ -5569,153 +5677,153 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:O27 J29:O29 J31:O75 J78:O97 J107:O112 J114:O1048576">
-    <cfRule type="cellIs" dxfId="40" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="50" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="52" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="53" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:O76">
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="38" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="39" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="40" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J77:O77">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J98:O103 J106:O106">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="30" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="32" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:O27 J29:O29 J31:O103 J106:O112 J114:O1048576">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:O30">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="21" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="22" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="23" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="24" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:O30">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:O28">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:O28">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J105:O105">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:O104">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:O105">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J113:O113">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J113:O113">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"check"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>